<commit_message>
Excel file with info on 42 buildings
</commit_message>
<xml_diff>
--- a/buildings.xlsx
+++ b/buildings.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$13</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="186">
   <si>
     <t>ID</t>
   </si>
@@ -193,13 +196,394 @@
   </si>
   <si>
     <t>Closed from 10AM-11AM every day, Breakfast 7:30-10, Lunch 11-5, Dinner 5-11(5-8 Friday Saturday)</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "address": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "S": "1809 N 13th St, Philadelphia, PA 19122"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "buildingname": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "SS": [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "tuttleman",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "tuttleman learning center",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "tuttleman center",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "tlc"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "hours": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "M": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "friday": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "S": "8 AM - 8 PM"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "monday": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "S": "8 AM - 9 PM"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "saturday": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "S": "closed"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "sunday": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "thursday": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "tuesday": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      "wednesday": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "id": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "N": "2"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  }</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>Liacouras Center</t>
+  </si>
+  <si>
+    <t>Liacouras Center Box Office</t>
+  </si>
+  <si>
+    <t>1776 N Broad St, Philadelphia, PA 19121</t>
+  </si>
+  <si>
+    <t>10 AM - 5 PM</t>
+  </si>
+  <si>
+    <t>(Hours vary)</t>
+  </si>
+  <si>
+    <t>http://www.liacourascenter.com/box-office-info</t>
+  </si>
+  <si>
+    <t>580 Meetinghouse Rd, Ambler, PA 19002</t>
+  </si>
+  <si>
+    <t>Temple Ambler Campus</t>
+  </si>
+  <si>
+    <t>https://ambler.temple.edu/students/computers-and-technology</t>
+  </si>
+  <si>
+    <t>8:30 AM - 10 PM</t>
+  </si>
+  <si>
+    <t>8:30 AM - 5 PM</t>
+  </si>
+  <si>
+    <t>NOON - 8 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3401 N Broad St, Philadelphia, PA 19140</t>
+  </si>
+  <si>
+    <t>1515 Market St. Philadelphia, PA 19102</t>
+  </si>
+  <si>
+    <t>Temple University Center City</t>
+  </si>
+  <si>
+    <t>Temple University Hospital</t>
+  </si>
+  <si>
+    <t>8:30 AM - 8 PM</t>
+  </si>
+  <si>
+    <t>Temple Performing Arts Center</t>
+  </si>
+  <si>
+    <t>Pearson and McGonigle Halls</t>
+  </si>
+  <si>
+    <t>O'Connot Plaza/Founder's Garden</t>
+  </si>
+  <si>
+    <t>Aramark STAR Complex</t>
+  </si>
+  <si>
+    <t>Beech International Village</t>
+  </si>
+  <si>
+    <t>1520 Cecil B Moore, Philadelphia, PA 19121</t>
+  </si>
+  <si>
+    <t>Cecil B Moore Subway Station</t>
+  </si>
+  <si>
+    <t>Edberg-Olson Football Practice Facility</t>
+  </si>
+  <si>
+    <t>Geasey Outdoor Field Complex</t>
+  </si>
+  <si>
+    <t>Johnson &amp; Hardwick Hall</t>
+  </si>
+  <si>
+    <t>Mitten Hall</t>
+  </si>
+  <si>
+    <t>Ritter Hall</t>
+  </si>
+  <si>
+    <t>The View</t>
+  </si>
+  <si>
+    <t>1837 N Broad St, Philadelphia, PA 19122</t>
+  </si>
+  <si>
+    <t>10 AM - 3 PM</t>
+  </si>
+  <si>
+    <t>1800 N. Broad St, Philadelphia, PA 19122</t>
+  </si>
+  <si>
+    <t>IBC Student Recreation Center</t>
+  </si>
+  <si>
+    <t>Temple University Fitness</t>
+  </si>
+  <si>
+    <t>Pearson &amp; McGonigle Halls Rec Courts</t>
+  </si>
+  <si>
+    <t>Pearson Hall Pool 31</t>
+  </si>
+  <si>
+    <t>Climbing Wall in Aramark  (STAR)  Complex</t>
+  </si>
+  <si>
+    <t>Weight Room in Aramark  (STAR)  Complex</t>
+  </si>
+  <si>
+    <t>12 PM - 8 PM</t>
+  </si>
+  <si>
+    <t>12 PM - 4 PM</t>
+  </si>
+  <si>
+    <t>6 AM - 11 PM</t>
+  </si>
+  <si>
+    <t>6 AM - 10 PM</t>
+  </si>
+  <si>
+    <t>9 AM - 8 PM</t>
+  </si>
+  <si>
+    <t>9 AM -10 PM</t>
+  </si>
+  <si>
+    <t>6:30am - 2:30pm and 5:00pm - 9:00pm</t>
+  </si>
+  <si>
+    <t>6:30am - 2:30pm and 5:00pm - 8:00pm</t>
+  </si>
+  <si>
+    <t>11:00am - 3:30pm</t>
+  </si>
+  <si>
+    <t>https://campusrecreation.temple.edu/hours-operation</t>
+  </si>
+  <si>
+    <t>11 am - 10 pm</t>
+  </si>
+  <si>
+    <t>12 pm - 8 pm</t>
+  </si>
+  <si>
+    <t>10 am - 10 pm</t>
+  </si>
+  <si>
+    <t>10 am - 9 pm</t>
+  </si>
+  <si>
+    <t>1 pm - 7pm</t>
+  </si>
+  <si>
+    <t>1 pm - 8pm</t>
+  </si>
+  <si>
+    <t>1100 W Montgomery Ave, Philadelphia, PA 19122</t>
+  </si>
+  <si>
+    <t>24 HOURS</t>
+  </si>
+  <si>
+    <t>Philadelphia, PA 19122</t>
+  </si>
+  <si>
+    <t>1816 N 15th St, Philadelphia, PA 19121</t>
+  </si>
+  <si>
+    <t>9 AM - 6 PM</t>
+  </si>
+  <si>
+    <t>1700 N. Broad St, Philadelphia, PA 19121</t>
+  </si>
+  <si>
+    <t>5 AM - 12 AM</t>
+  </si>
+  <si>
+    <t>McDonalds</t>
+  </si>
+  <si>
+    <t>2109 N Broad St, Philadelphia, PA 19122</t>
+  </si>
+  <si>
+    <t>1001 Diamond St, Philadelphia, PA 19122</t>
+  </si>
+  <si>
+    <t>hours may vary</t>
+  </si>
+  <si>
+    <t>1890 N 15th St, Philadelphia, PA 19121</t>
+  </si>
+  <si>
+    <t>hours vary based on events</t>
+  </si>
+  <si>
+    <t>J&amp;H Dining Hall</t>
+  </si>
+  <si>
+    <t>2029 N Broad St, Philadelphia, PA 19122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 AM - 8 PM </t>
+  </si>
+  <si>
+    <t>8 AM -  8 PM</t>
+  </si>
+  <si>
+    <t>8 AM - 12 AM</t>
+  </si>
+  <si>
+    <t>Wendy's</t>
+  </si>
+  <si>
+    <t>Burger King</t>
+  </si>
+  <si>
+    <t>Beasley School of Law</t>
+  </si>
+  <si>
+    <t>1719 N Broad St, Philadelphia, PA 19122</t>
+  </si>
+  <si>
+    <t>8 am - 11 pm</t>
+  </si>
+  <si>
+    <t>1600 N Broad St, Philadelphia, PA 19121</t>
+  </si>
+  <si>
+    <t>Temple University, 1913, N Broad St, Philadelphia, PA 19122</t>
+  </si>
+  <si>
+    <t> 2001 N 13th St, Philadelphia, PA 19122</t>
+  </si>
+  <si>
+    <t>Boyer College of Music and Dance/Presser Hall</t>
+  </si>
+  <si>
+    <t>1301 Cecil B. Moore Ave, Philadelphia, PA 19122</t>
+  </si>
+  <si>
+    <t>8 AM - 4:30 PM</t>
+  </si>
+  <si>
+    <t>Draught Horse</t>
+  </si>
+  <si>
+    <t>Philly Style Pizza</t>
+  </si>
+  <si>
+    <t>1708 N Broad St, Philadelphia, PA 19121</t>
+  </si>
+  <si>
+    <t>10 AM - 1 AM</t>
+  </si>
+  <si>
+    <t>10 AM - 2 AM</t>
+  </si>
+  <si>
+    <t>1431 Cecil B. Moore Ave, Philadelphia, PA 19121</t>
+  </si>
+  <si>
+    <t>11:30 am - 12 am</t>
+  </si>
+  <si>
+    <t>11:30 am - 2 am</t>
+  </si>
+  <si>
+    <t>11:30 am - 11 pm</t>
+  </si>
+  <si>
+    <t>2010 N Broad St, Philadelphia, PA 19121</t>
+  </si>
+  <si>
+    <t>11 am - 11 pm</t>
+  </si>
+  <si>
+    <t>11 am - 3 am</t>
+  </si>
+  <si>
+    <t>12 pm - 11 pm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +598,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF303030"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -237,7 +639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -246,6 +648,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -548,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,392 +1024,1487 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K7" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="8" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="M9" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="K12" s="5"/>
+      <c r="M12" s="6" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>58</v>
+      <c r="B15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M13">
+    <sortState ref="A2:M13">
+      <sortCondition ref="A1:A13"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="M7" r:id="rId1" tooltip="Call via Hangouts" display="https://www.google.com/search?q=temple+campus+safety+services&amp;oq=temple+campus+safety+services&amp;aqs=chrome..69i57j0.4177j0j7&amp;sourceid=chrome&amp;ie=UTF-8"/>
-    <hyperlink ref="M9" r:id="rId2" tooltip="Call via Hangouts" display="https://www.google.com/search?q=temple+alter+hall&amp;oq=temple+alter+hall&amp;aqs=chrome..69i57j0l5.2566j0j7&amp;sourceid=chrome&amp;ie=UTF-8"/>
-    <hyperlink ref="M10" r:id="rId3" tooltip="Call via Hangouts" display="https://www.google.com/search?safe=active&amp;ei=9BKoXIjIG8iw5wLT-YqYCg&amp;q=temple+science+education+and+research+center+&amp;oq=temple+science+education+and+research+center+&amp;gs_l=psy-ab.3..0i22i30j38.8896.14435..15361...3.0..0.118.1564.19j1....2..0....1..gws-wiz.....6..0i71j35i39j0i273j0i67j0i131i273j0j0i20i263j0i10.DZ8YZgN12xo"/>
+    <hyperlink ref="M12" r:id="rId1" tooltip="Call via Hangouts" display="https://www.google.com/search?q=temple+campus+safety+services&amp;oq=temple+campus+safety+services&amp;aqs=chrome..69i57j0.4177j0j7&amp;sourceid=chrome&amp;ie=UTF-8"/>
+    <hyperlink ref="M2" r:id="rId2" tooltip="Call via Hangouts" display="https://www.google.com/search?q=temple+alter+hall&amp;oq=temple+alter+hall&amp;aqs=chrome..69i57j0l5.2566j0j7&amp;sourceid=chrome&amp;ie=UTF-8"/>
+    <hyperlink ref="M9" r:id="rId3" tooltip="Call via Hangouts" display="https://www.google.com/search?safe=active&amp;ei=9BKoXIjIG8iw5wLT-YqYCg&amp;q=temple+science+education+and+research+center+&amp;oq=temple+science+education+and+research+center+&amp;gs_l=psy-ab.3..0i22i30j38.8896.14435..15361...3.0..0.118.1564.19j1....2..0....1..gws-wiz.....6..0i71j35i39j0i273j0i67j0i131i273j0j0i20i263j0i10.DZ8YZgN12xo"/>
+    <hyperlink ref="K15" r:id="rId4"/>
+    <hyperlink ref="K16" r:id="rId5"/>
+    <hyperlink ref="K24" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:A41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>